<commit_message>
Se agrega opciones para sotrage types de MP y MP1
</commit_message>
<xml_diff>
--- a/Programa_RAW.xlsx
+++ b/Programa_RAW.xlsx
@@ -29,16 +29,16 @@
     <t>numero_sap</t>
   </si>
   <si>
-    <t>1000009307A0</t>
-  </si>
-  <si>
     <t>contenedores</t>
   </si>
   <si>
-    <t>1000009293A0</t>
+    <t>1000009457A0</t>
   </si>
   <si>
-    <t>1000009295A0</t>
+    <t>1000011685A0</t>
+  </si>
+  <si>
+    <t>1000013744A0</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1048576"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,20 +391,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
         <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
@@ -412,7 +412,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>

</xml_diff>